<commit_message>
Changed file directories to reflect folder changes
</commit_message>
<xml_diff>
--- a/DataTables/ExtractedAllbyDV.xlsx
+++ b/DataTables/ExtractedAllbyDV.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rutgersconnect-my.sharepoint.com/personal/hg284_shp_rutgers_edu/Documents/thesis_stuff/data/DataProcessing/Gorin CMBN F4 project/DataTables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rutgersconnect-my.sharepoint.com/personal/hg284_shp_rutgers_edu/Documents/thesis_stuff/data/DataProcessing/gorin_CMBN_F4_project/DataTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{502F8A53-160F-8842-9766-0CD01516E902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{027F995C-30A8-9147-B777-25E92D6236AE}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{502F8A53-160F-8842-9766-0CD01516E902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A3DD9B92-A1B8-5E48-AB65-A64CD356C5C0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16760" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="epoch" sheetId="1" r:id="rId1"/>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4319,7 +4319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>

</xml_diff>